<commit_message>
Agregue envio a correo.
</commit_message>
<xml_diff>
--- a/Changarro/ChangarroManager/Plantillas/PlantillaVacia/Plantilla.xlsx
+++ b/Changarro/ChangarroManager/Plantillas/PlantillaVacia/Plantilla.xlsx
@@ -78,6 +78,14 @@
     <sheetView tabSelected="1" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Requerimientos 1 y 2
</commit_message>
<xml_diff>
--- a/Changarro/ChangarroManager/Plantillas/PlantillaVacia/Plantilla.xlsx
+++ b/Changarro/ChangarroManager/Plantillas/PlantillaVacia/Plantilla.xlsx
@@ -78,6 +78,14 @@
     <sheetView tabSelected="1" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Ultimas modificaciones y comentarios.
</commit_message>
<xml_diff>
--- a/Changarro/ChangarroManager/Plantillas/PlantillaVacia/Plantilla.xlsx
+++ b/Changarro/ChangarroManager/Plantillas/PlantillaVacia/Plantilla.xlsx
@@ -7,6 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="1" r:id="rId3"/>
+    <sheet name="Categorias" sheetId="2" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -65,8 +66,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -88,26 +92,46 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations disablePrompts="0" count="2">
+    <dataValidation type="list" errorStyle="stop" imeMode="noControl" operator="between" allowBlank="1" showDropDown="0" showInputMessage="0" showErrorMessage="0" sqref="D2:D301">
+      <formula1><![CDATA["Moda,Tecnologia,Joyas y Relojes,Belleza,Infantil,Deportes y Fitness,Vehículos,Hogar,VideosJuegos,Mascotas"]]></formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="stop" imeMode="noControl" operator="between" allowBlank="1" showDropDown="0" showInputMessage="0" showErrorMessage="0" sqref="E2:E301">
+      <formula1><![CDATA["Activo,Inactivo"]]></formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>